<commit_message>
Small fix to the ER contribution hitorical numbers
</commit_message>
<xml_diff>
--- a/Model Inputs 2021.xlsx
+++ b/Model Inputs 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongbui/Dropbox/Career management/Reason/Reason Work/R projects/Plan Models/North Dakota PERS/NDPERS-Funding Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF5FC7-441C-C34A-9683-DAD7EC2A3BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7202D48-754D-814B-B800-CC96C7C30905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5404,8 +5404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:DB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="BA3" sqref="BA3"/>
+    <sheetView tabSelected="1" topLeftCell="BW1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="CE6" sqref="CE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6059,10 +6059,11 @@
       </c>
       <c r="CD2" s="38">
         <f>CE2+AI2</f>
-        <v>974.59747700000025</v>
+        <v>1047.5579650000002</v>
       </c>
       <c r="CE2" s="9">
-        <v>0</v>
+        <f>CC2</f>
+        <v>72.960487999999998</v>
       </c>
       <c r="CF2" s="9">
         <v>0</v>
@@ -6354,17 +6355,18 @@
         <v>74.023555000000002</v>
       </c>
       <c r="CE3" s="9">
-        <v>0</v>
+        <f t="shared" ref="CE3:CE7" si="3">CC3</f>
+        <v>74.023555000000002</v>
       </c>
       <c r="CF3" s="9">
         <v>0</v>
       </c>
       <c r="CG3" s="10">
-        <f t="shared" ref="CG3:CG7" si="3">CC3/B3</f>
+        <f t="shared" ref="CG3:CG7" si="4">CC3/B3</f>
         <v>7.251216558709038E-2</v>
       </c>
       <c r="CH3" s="61">
-        <f t="shared" ref="CH3:CH6" si="4">BD3+BJ3+BI3+BL3+BN3+BS3+BU3+BR3+BP3</f>
+        <f t="shared" ref="CH3:CH6" si="5">BD3+BJ3+BI3+BL3+BN3+BS3+BU3+BR3+BP3</f>
         <v>-3.9957620000000009</v>
       </c>
       <c r="CI3" s="62">
@@ -6388,15 +6390,15 @@
         <v>0</v>
       </c>
       <c r="CN3" s="62">
-        <f t="shared" ref="CN3:CP3" si="5">CM2</f>
+        <f t="shared" ref="CN3:CP3" si="6">CM2</f>
         <v>0</v>
       </c>
       <c r="CO3" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CP3" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CQ3" s="62">
@@ -6404,7 +6406,7 @@
         <v>22.7863915678744</v>
       </c>
       <c r="CR3" s="34">
-        <f t="shared" ref="CR3:CR6" si="6">BE3+BK3+BM3+BO3+BT3+BR3+BQ3+BV3</f>
+        <f t="shared" ref="CR3:CR6" si="7">BE3+BK3+BM3+BO3+BT3+BR3+BQ3+BV3</f>
         <v>0</v>
       </c>
       <c r="CS3">
@@ -6662,57 +6664,58 @@
         <v>75.666300000000007</v>
       </c>
       <c r="CE4" s="9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>75.666300000000007</v>
       </c>
       <c r="CF4" s="9">
         <v>0</v>
       </c>
       <c r="CG4" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.3654271390269199E-2</v>
       </c>
       <c r="CH4" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-9.8985329999999792</v>
       </c>
       <c r="CI4" s="62">
-        <f t="shared" ref="CI4:CI7" si="7">AC3*L3+CH4*((1+L3)^0.5-1)</f>
+        <f t="shared" ref="CI4:CI7" si="8">AC3*L3+CH4*((1+L3)^0.5-1)</f>
         <v>202.71588459451851</v>
       </c>
       <c r="CJ4" s="62">
-        <f t="shared" ref="CJ4:CJ6" si="8">AC3+CH4+CI4</f>
+        <f t="shared" ref="CJ4:CJ6" si="9">AC3+CH4+CI4</f>
         <v>2813.3631045945185</v>
       </c>
       <c r="CK4" s="62">
-        <f t="shared" ref="CK4:CK6" si="9">AC4-CJ4</f>
+        <f t="shared" ref="CK4:CK6" si="10">AC4-CJ4</f>
         <v>35.955970405481366</v>
       </c>
       <c r="CL4" s="62">
-        <f t="shared" ref="CL4:CL7" si="10">CK4*0.2</f>
+        <f t="shared" ref="CL4:CL7" si="11">CK4*0.2</f>
         <v>7.191194081096274</v>
       </c>
       <c r="CM4" s="62">
-        <f t="shared" ref="CM4:CP7" si="11">CL3</f>
+        <f t="shared" ref="CM4:CP7" si="12">CL3</f>
         <v>22.7863915678744</v>
       </c>
       <c r="CN4" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CO4" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CP4" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CQ4" s="62">
-        <f t="shared" ref="CQ4:CQ7" si="12">SUM(CL4:CP4)</f>
+        <f t="shared" ref="CQ4:CQ7" si="13">SUM(CL4:CP4)</f>
         <v>29.977585648970674</v>
       </c>
       <c r="CR4" s="34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CS4">
@@ -6972,57 +6975,58 @@
         <v>75.730260000000001</v>
       </c>
       <c r="CE5" s="9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>75.730260000000001</v>
       </c>
       <c r="CF5" s="9">
         <v>0</v>
       </c>
       <c r="CG5" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.2805644588690155E-2</v>
       </c>
       <c r="CH5" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-36.581496999999999</v>
       </c>
       <c r="CI5" s="62">
+        <f t="shared" si="8"/>
+        <v>219.43114465520219</v>
+      </c>
+      <c r="CJ5" s="62">
+        <f t="shared" si="9"/>
+        <v>3032.1687226552021</v>
+      </c>
+      <c r="CK5" s="62">
+        <f t="shared" si="10"/>
+        <v>-67.988094655202076</v>
+      </c>
+      <c r="CL5" s="62">
+        <f t="shared" si="11"/>
+        <v>-13.597618931040415</v>
+      </c>
+      <c r="CM5" s="62">
+        <f t="shared" si="12"/>
+        <v>7.191194081096274</v>
+      </c>
+      <c r="CN5" s="62">
+        <f t="shared" si="12"/>
+        <v>22.7863915678744</v>
+      </c>
+      <c r="CO5" s="62">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="CP5" s="62">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="62">
+        <f t="shared" si="13"/>
+        <v>16.379966717930259</v>
+      </c>
+      <c r="CR5" s="34">
         <f t="shared" si="7"/>
-        <v>219.43114465520219</v>
-      </c>
-      <c r="CJ5" s="62">
-        <f t="shared" si="8"/>
-        <v>3032.1687226552021</v>
-      </c>
-      <c r="CK5" s="62">
-        <f t="shared" si="9"/>
-        <v>-67.988094655202076</v>
-      </c>
-      <c r="CL5" s="62">
-        <f t="shared" si="10"/>
-        <v>-13.597618931040415</v>
-      </c>
-      <c r="CM5" s="62">
-        <f t="shared" si="11"/>
-        <v>7.191194081096274</v>
-      </c>
-      <c r="CN5" s="62">
-        <f t="shared" si="11"/>
-        <v>22.7863915678744</v>
-      </c>
-      <c r="CO5" s="62">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CP5" s="62">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CQ5" s="62">
-        <f t="shared" si="12"/>
-        <v>16.379966717930259</v>
-      </c>
-      <c r="CR5" s="34">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CS5">
@@ -7288,57 +7292,58 @@
         <v>78.110561000000004</v>
       </c>
       <c r="CE6" s="9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>78.110561000000004</v>
       </c>
       <c r="CF6" s="9">
         <v>0</v>
       </c>
       <c r="CG6" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.0808716965289759E-2</v>
       </c>
       <c r="CH6" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-49.068123000000014</v>
       </c>
       <c r="CI6" s="62">
+        <f t="shared" si="8"/>
+        <v>220.50675735463145</v>
+      </c>
+      <c r="CJ6" s="62">
+        <f t="shared" si="9"/>
+        <v>3135.6192623546317</v>
+      </c>
+      <c r="CK6" s="62">
+        <f t="shared" si="10"/>
+        <v>-124.11996835463151</v>
+      </c>
+      <c r="CL6" s="62">
+        <f t="shared" si="11"/>
+        <v>-24.823993670926303</v>
+      </c>
+      <c r="CM6" s="62">
+        <f t="shared" si="12"/>
+        <v>-13.597618931040415</v>
+      </c>
+      <c r="CN6" s="62">
+        <f t="shared" si="12"/>
+        <v>7.191194081096274</v>
+      </c>
+      <c r="CO6" s="62">
+        <f t="shared" si="12"/>
+        <v>22.7863915678744</v>
+      </c>
+      <c r="CP6" s="62">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="CQ6" s="62">
+        <f t="shared" si="13"/>
+        <v>-8.4440269529960403</v>
+      </c>
+      <c r="CR6" s="34">
         <f t="shared" si="7"/>
-        <v>220.50675735463145</v>
-      </c>
-      <c r="CJ6" s="62">
-        <f t="shared" si="8"/>
-        <v>3135.6192623546317</v>
-      </c>
-      <c r="CK6" s="62">
-        <f t="shared" si="9"/>
-        <v>-124.11996835463151</v>
-      </c>
-      <c r="CL6" s="62">
-        <f t="shared" si="10"/>
-        <v>-24.823993670926303</v>
-      </c>
-      <c r="CM6" s="62">
-        <f t="shared" si="11"/>
-        <v>-13.597618931040415</v>
-      </c>
-      <c r="CN6" s="62">
-        <f t="shared" si="11"/>
-        <v>7.191194081096274</v>
-      </c>
-      <c r="CO6" s="62">
-        <f t="shared" si="11"/>
-        <v>22.7863915678744</v>
-      </c>
-      <c r="CP6" s="62">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="CQ6" s="62">
-        <f t="shared" si="12"/>
-        <v>-8.4440269529960403</v>
-      </c>
-      <c r="CR6" s="34">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CS6">
@@ -7623,57 +7628,58 @@
         <v>80.844430634999995</v>
       </c>
       <c r="CE7" s="9">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>80.844430634999995</v>
       </c>
       <c r="CF7" s="9">
         <v>0</v>
       </c>
       <c r="CG7" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.1392698581927108E-2</v>
       </c>
       <c r="CH7" s="61">
-        <f t="shared" ref="CH7" si="13">BD7+BJ7+BI7+BL7+BN7+BS7+BU7+BR7+BP7</f>
+        <f t="shared" ref="CH7" si="14">BD7+BJ7+BI7+BL7+BN7+BS7+BU7+BR7+BP7</f>
         <v>-53.821427899692786</v>
       </c>
       <c r="CI7" s="62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>208.95306055949735</v>
       </c>
       <c r="CJ7" s="62">
-        <f t="shared" ref="CJ7" si="14">AC6+CH7+CI7</f>
+        <f t="shared" ref="CJ7" si="15">AC6+CH7+CI7</f>
         <v>3166.6309266598046</v>
       </c>
       <c r="CK7" s="62">
-        <f t="shared" ref="CK7" si="15">AC7-CJ7</f>
+        <f t="shared" ref="CK7" si="16">AC7-CJ7</f>
         <v>586.1226853401954</v>
       </c>
       <c r="CL7" s="62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>117.22453706803908</v>
       </c>
       <c r="CM7" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-24.823993670926303</v>
       </c>
       <c r="CN7" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-13.597618931040415</v>
       </c>
       <c r="CO7" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.191194081096274</v>
       </c>
       <c r="CP7" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>22.7863915678744</v>
       </c>
       <c r="CQ7" s="62">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>108.78051011504304</v>
       </c>
       <c r="CR7" s="34">
-        <f t="shared" ref="CR7" si="16">BE7+BK7+BM7+BO7+BT7+BR7+BQ7+BV7</f>
+        <f t="shared" ref="CR7" si="17">BE7+BK7+BM7+BO7+BT7+BR7+BQ7+BV7</f>
         <v>0</v>
       </c>
       <c r="CS7">

</xml_diff>